<commit_message>
addressed many FJM comments in text
</commit_message>
<xml_diff>
--- a/Ch1_Tables.xlsx
+++ b/Ch1_Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\Desktop\Grad School\Thesis2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtpriest\Desktop\GradSchool\Thesis2019_Ch1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D6B628-1AFA-440C-8867-B314530D6991}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BC230F-8AF4-481D-A02B-6E77F9CC32D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EC0383BB-9F3C-437D-BF2A-12F22EF652FA}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EC0383BB-9F3C-437D-BF2A-12F22EF652FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Table2_V2" sheetId="4" r:id="rId4"/>
     <sheet name="Table2_V3" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -500,7 +501,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -546,6 +547,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -872,18 +882,18 @@
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.28515625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="27.33203125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" style="5" customWidth="1"/>
     <col min="12" max="12" width="12" style="5" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" style="5" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" customWidth="1"/>
+    <col min="13" max="13" width="12.5546875" style="5" customWidth="1"/>
+    <col min="14" max="14" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -925,7 +935,7 @@
       </c>
       <c r="O1" s="7"/>
     </row>
-    <row r="2" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -971,7 +981,7 @@
       </c>
       <c r="O2" s="7"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1015,7 +1025,7 @@
       </c>
       <c r="O3" s="7"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1059,7 +1069,7 @@
       </c>
       <c r="O4" s="7"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1103,7 +1113,7 @@
       </c>
       <c r="O5" s="7"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1147,7 +1157,7 @@
       </c>
       <c r="O6" s="7"/>
     </row>
-    <row r="7" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1193,7 +1203,7 @@
       </c>
       <c r="O7" s="7"/>
     </row>
-    <row r="8" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1239,7 +1249,7 @@
       </c>
       <c r="O8" s="7"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1283,7 +1293,7 @@
       </c>
       <c r="O9" s="7"/>
     </row>
-    <row r="10" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1329,7 +1339,7 @@
       </c>
       <c r="O10" s="7"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1373,7 +1383,7 @@
       </c>
       <c r="O11" s="7"/>
     </row>
-    <row r="12" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1419,7 +1429,7 @@
       </c>
       <c r="O12" s="7"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1463,7 +1473,7 @@
       </c>
       <c r="O13" s="7"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1507,7 +1517,7 @@
       </c>
       <c r="O14" s="7"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1551,7 +1561,7 @@
       </c>
       <c r="O15" s="7"/>
     </row>
-    <row r="16" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1597,7 +1607,7 @@
       </c>
       <c r="O16" s="7"/>
     </row>
-    <row r="17" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1643,7 +1653,7 @@
       </c>
       <c r="O17" s="7"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1687,7 +1697,7 @@
       </c>
       <c r="O18" s="7"/>
     </row>
-    <row r="19" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1733,7 +1743,7 @@
       </c>
       <c r="O19" s="7"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1777,7 +1787,7 @@
       </c>
       <c r="O20" s="7"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1821,7 +1831,7 @@
       </c>
       <c r="O21" s="7"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1865,7 +1875,7 @@
       </c>
       <c r="O22" s="7"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1909,7 +1919,7 @@
       </c>
       <c r="O23" s="7"/>
     </row>
-    <row r="24" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1955,7 +1965,7 @@
       </c>
       <c r="O24" s="7"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1999,7 +2009,7 @@
       </c>
       <c r="O25" s="7"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -2043,7 +2053,7 @@
       </c>
       <c r="O26" s="7"/>
     </row>
-    <row r="27" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -2089,7 +2099,7 @@
       </c>
       <c r="O27" s="7"/>
     </row>
-    <row r="28" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -2135,7 +2145,7 @@
       </c>
       <c r="O28" s="7"/>
     </row>
-    <row r="29" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -2181,7 +2191,7 @@
       </c>
       <c r="O29" s="7"/>
     </row>
-    <row r="30" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -2227,7 +2237,7 @@
       </c>
       <c r="O30" s="7"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -2271,7 +2281,7 @@
       </c>
       <c r="O31" s="7"/>
     </row>
-    <row r="32" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -2317,21 +2327,21 @@
       </c>
       <c r="O32" s="7"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="N34" s="7"/>
       <c r="O34" s="7"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="K36" s="6">
         <f>SUM(K2:K32)</f>
         <v>1784593</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -2354,7 +2364,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -2374,7 +2384,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -2394,7 +2404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -2414,7 +2424,7 @@
         <v>0.89600000000000002</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -2434,7 +2444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>11</v>
       </c>
@@ -2454,7 +2464,7 @@
         <v>0.46400000000000002</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>12</v>
       </c>
@@ -2474,7 +2484,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>13</v>
       </c>
@@ -2494,7 +2504,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>14</v>
       </c>
@@ -2514,7 +2524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -2534,7 +2544,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>16</v>
       </c>
@@ -2554,7 +2564,7 @@
         <v>0.311</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>17</v>
       </c>
@@ -2574,7 +2584,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -2594,7 +2604,7 @@
         <v>0.98899999999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>19</v>
       </c>
@@ -2614,7 +2624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>20</v>
       </c>
@@ -2634,7 +2644,7 @@
         <v>0.97899999999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>21</v>
       </c>
@@ -2654,7 +2664,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>22</v>
       </c>
@@ -2674,7 +2684,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>23</v>
       </c>
@@ -2694,7 +2704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>24</v>
       </c>
@@ -2714,7 +2724,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>25</v>
       </c>
@@ -2734,7 +2744,7 @@
         <v>0.754</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>26</v>
       </c>
@@ -2754,7 +2764,7 @@
         <v>0.34599999999999997</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>27</v>
       </c>
@@ -2774,7 +2784,7 @@
         <v>0.36099999999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>28</v>
       </c>
@@ -2794,7 +2804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>29</v>
       </c>
@@ -2814,7 +2824,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>30</v>
       </c>
@@ -2834,7 +2844,7 @@
         <v>0.68600000000000005</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>31</v>
       </c>
@@ -2854,7 +2864,7 @@
         <v>0.96799999999999997</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>32</v>
       </c>
@@ -2874,7 +2884,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>33</v>
       </c>
@@ -2894,7 +2904,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>34</v>
       </c>
@@ -2914,7 +2924,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>35</v>
       </c>
@@ -2934,7 +2944,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>36</v>
       </c>
@@ -2954,7 +2964,7 @@
         <v>0.36099999999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>37</v>
       </c>
@@ -2988,14 +2998,14 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3015,7 +3025,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -3038,7 +3048,7 @@
         <v>1784593</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3057,7 +3067,7 @@
         <v>0.47428293173849723</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -3076,7 +3086,7 @@
         <v>0.60372421050626102</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3095,7 +3105,7 @@
         <v>0.70588924197281955</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -3114,7 +3124,7 @@
         <v>0.8024434703038732</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -3133,7 +3143,7 @@
         <v>0.88086583327402945</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -3152,7 +3162,7 @@
         <v>0.92425555855032493</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -3171,7 +3181,7 @@
         <v>0.9526743632861947</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -3190,7 +3200,7 @@
         <v>0.97092782499987396</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -3209,7 +3219,7 @@
         <v>0.98888990374836172</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -3228,7 +3238,7 @@
         <v>0.9939235444720449</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -3247,7 +3257,7 @@
         <v>0.99802419935525921</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -3266,7 +3276,7 @@
         <v>0.99855653361858987</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -3285,7 +3295,7 @@
         <v>0.99903003093702603</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -3304,7 +3314,7 @@
         <v>0.99935335395801739</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -3323,7 +3333,7 @@
         <v>0.99965034044177026</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -3342,7 +3352,7 @@
         <v>0.99992323179570919</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -3361,7 +3371,7 @@
         <v>0.99995293044408451</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -3380,7 +3390,7 @@
         <v>0.99997086170348093</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -3399,7 +3409,7 @@
         <v>0.99998150838874755</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>86</v>
       </c>
@@ -3418,7 +3428,7 @@
         <v>0.9999865515554528</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -3437,7 +3447,7 @@
         <v>0.99998991366658962</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -3456,7 +3466,7 @@
         <v>0.99999215507401418</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>80</v>
       </c>
@@ -3475,7 +3485,7 @@
         <v>0.99999383612958259</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>91</v>
       </c>
@@ -3494,7 +3504,7 @@
         <v>0.99999495683329487</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>88</v>
       </c>
@@ -3513,7 +3523,7 @@
         <v>0.99999607753700714</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>87</v>
       </c>
@@ -3532,7 +3542,7 @@
         <v>0.99999719824071942</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -3551,7 +3561,7 @@
         <v>0.9999983189444317</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>90</v>
       </c>
@@ -3570,7 +3580,7 @@
         <v>0.99999887929628783</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>85</v>
       </c>
@@ -3589,7 +3599,7 @@
         <v>0.99999943964814397</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -3609,7 +3619,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C32">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C32">
     <sortCondition descending="1" ref="C2:C32"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3621,23 +3631,23 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" style="5" customWidth="1"/>
-    <col min="3" max="4" width="8.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="1.42578125" style="5" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="1.42578125" style="5" customWidth="1"/>
-    <col min="9" max="10" width="8.7109375" style="5" customWidth="1"/>
-    <col min="11" max="11" width="1.42578125" style="5" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="4.44140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" style="5" customWidth="1"/>
+    <col min="3" max="4" width="8.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="1.44140625" style="5" customWidth="1"/>
+    <col min="6" max="7" width="9.109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="1.44140625" style="5" customWidth="1"/>
+    <col min="9" max="10" width="8.6640625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="2.33203125" style="5" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="11"/>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -3653,31 +3663,31 @@
       <c r="M1" s="11"/>
       <c r="N1" s="11"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="25"/>
+      <c r="D2" s="28"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="G2" s="25"/>
+      <c r="G2" s="28"/>
       <c r="H2" s="11"/>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="J2" s="25"/>
+      <c r="J2" s="28"/>
       <c r="K2" s="11"/>
-      <c r="L2" s="25" t="s">
+      <c r="L2" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="M2" s="25"/>
+      <c r="M2" s="28"/>
       <c r="N2" s="11"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="8" t="s">
         <v>0</v>
@@ -3702,7 +3712,7 @@
       <c r="J3" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="K3" s="8"/>
+      <c r="K3" s="11"/>
       <c r="L3" s="18" t="s">
         <v>115</v>
       </c>
@@ -3711,7 +3721,7 @@
       </c>
       <c r="N3" s="11"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="11" t="s">
         <v>8</v>
@@ -3730,10 +3740,10 @@
         <v>0.78900000000000003</v>
       </c>
       <c r="H4" s="15"/>
-      <c r="I4" s="14">
+      <c r="I4" s="19">
         <v>161.9</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="25" t="s">
         <v>120</v>
       </c>
       <c r="K4" s="11"/>
@@ -3745,15 +3755,15 @@
       </c>
       <c r="N4" s="11"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="19">
         <v>-813.7</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="25">
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="E5" s="15"/>
@@ -3782,7 +3792,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="11" t="s">
         <v>10</v>
@@ -3794,10 +3804,10 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="E6" s="15"/>
-      <c r="F6" s="14">
+      <c r="F6" s="19">
         <v>128.69999999999999</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="25" t="s">
         <v>120</v>
       </c>
       <c r="H6" s="15"/>
@@ -3816,7 +3826,7 @@
       </c>
       <c r="N6" s="11"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="11" t="s">
         <v>11</v>
@@ -3850,22 +3860,22 @@
       </c>
       <c r="N7" s="11"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="19">
         <v>44.3</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="25" t="s">
         <v>120</v>
       </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="14">
+      <c r="F8" s="19">
         <v>148.80000000000001</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="25" t="s">
         <v>120</v>
       </c>
       <c r="H8" s="15"/>
@@ -3884,7 +3894,7 @@
       </c>
       <c r="N8" s="11"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="11" t="s">
         <v>16</v>
@@ -3903,10 +3913,10 @@
         <v>0.64300000000000002</v>
       </c>
       <c r="H9" s="15"/>
-      <c r="I9" s="14">
+      <c r="I9" s="19">
         <v>1</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="25">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="K9" s="11"/>
@@ -3918,7 +3928,7 @@
       </c>
       <c r="N9" s="11"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="11" t="s">
         <v>18</v>
@@ -3930,44 +3940,44 @@
         <v>0.76400000000000001</v>
       </c>
       <c r="E10" s="15"/>
-      <c r="F10" s="14">
+      <c r="F10" s="19">
         <v>-45.9</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="25" t="s">
         <v>120</v>
       </c>
       <c r="H10" s="15"/>
-      <c r="I10" s="14">
+      <c r="I10" s="19">
         <v>-7.9</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="25">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="K10" s="11"/>
-      <c r="L10" s="24">
+      <c r="L10" s="26">
         <v>0.03</v>
       </c>
-      <c r="M10" s="15">
+      <c r="M10" s="27">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="N10" s="11"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="19">
         <v>-18.100000000000001</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="25">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E11" s="15"/>
-      <c r="F11" s="14">
+      <c r="F11" s="19">
         <v>43.5</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="25">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="H11" s="15"/>
@@ -3986,15 +3996,15 @@
       </c>
       <c r="N11" s="11"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="19">
         <v>-3.9</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="25">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="E12" s="15"/>
@@ -4005,10 +4015,10 @@
         <v>0.875</v>
       </c>
       <c r="H12" s="15"/>
-      <c r="I12" s="14">
+      <c r="I12" s="19">
         <v>-5.4</v>
       </c>
-      <c r="J12" s="20">
+      <c r="J12" s="25">
         <v>2E-3</v>
       </c>
       <c r="K12" s="11"/>
@@ -4020,15 +4030,15 @@
       </c>
       <c r="N12" s="11"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="19">
         <v>-90.3</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="25" t="s">
         <v>120</v>
       </c>
       <c r="E13" s="15"/>
@@ -4039,10 +4049,10 @@
         <v>0.40200000000000002</v>
       </c>
       <c r="H13" s="15"/>
-      <c r="I13" s="14">
+      <c r="I13" s="19">
         <v>-61</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="J13" s="25" t="s">
         <v>120</v>
       </c>
       <c r="K13" s="11"/>
@@ -4054,7 +4064,7 @@
       </c>
       <c r="N13" s="11"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="11" t="s">
         <v>25</v>
@@ -4088,7 +4098,7 @@
       </c>
       <c r="N14" s="11"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="11" t="s">
         <v>26</v>
@@ -4107,10 +4117,10 @@
         <v>0.56799999999999995</v>
       </c>
       <c r="H15" s="15"/>
-      <c r="I15" s="14">
+      <c r="I15" s="19">
         <v>0.4</v>
       </c>
-      <c r="J15" s="20" t="s">
+      <c r="J15" s="25" t="s">
         <v>120</v>
       </c>
       <c r="K15" s="11"/>
@@ -4122,7 +4132,7 @@
       </c>
       <c r="N15" s="11"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="11" t="s">
         <v>27</v>
@@ -4156,7 +4166,7 @@
       </c>
       <c r="N16" s="11"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="11" t="s">
         <v>28</v>
@@ -4190,7 +4200,7 @@
       </c>
       <c r="N17" s="11"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="11" t="s">
         <v>30</v>
@@ -4224,41 +4234,41 @@
       </c>
       <c r="N18" s="11"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
       <c r="B19" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="19">
         <v>13.6</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="25">
         <v>1.4E-2</v>
       </c>
       <c r="E19" s="15"/>
-      <c r="F19" s="14">
+      <c r="F19" s="19">
         <v>50.4</v>
       </c>
-      <c r="G19" s="20">
+      <c r="G19" s="25">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="H19" s="15"/>
-      <c r="I19" s="14">
+      <c r="I19" s="19">
         <v>17.600000000000001</v>
       </c>
-      <c r="J19" s="20">
+      <c r="J19" s="25">
         <v>2E-3</v>
       </c>
       <c r="K19" s="11"/>
-      <c r="L19" s="24">
+      <c r="L19" s="26">
         <v>-0.04</v>
       </c>
-      <c r="M19" s="15">
+      <c r="M19" s="27">
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="N19" s="11"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" s="11" t="s">
         <v>36</v>
@@ -4292,7 +4302,7 @@
       </c>
       <c r="N20" s="11"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -4308,7 +4318,7 @@
       <c r="M21" s="11"/>
       <c r="N21" s="11"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -4344,19 +4354,19 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="1.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="4.44140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="1.44140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.44140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="11"/>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -4366,7 +4376,7 @@
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="18" t="s">
@@ -4382,7 +4392,7 @@
       </c>
       <c r="H2" s="11"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="8" t="s">
         <v>0</v>
@@ -4400,7 +4410,7 @@
       </c>
       <c r="H3" s="11"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="11" t="s">
         <v>8</v>
@@ -4418,7 +4428,7 @@
       </c>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="11" t="s">
         <v>9</v>
@@ -4436,7 +4446,7 @@
       </c>
       <c r="H5" s="11"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="11" t="s">
         <v>10</v>
@@ -4454,7 +4464,7 @@
       </c>
       <c r="H6" s="11"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="11" t="s">
         <v>14</v>
@@ -4472,7 +4482,7 @@
       </c>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="11" t="s">
         <v>16</v>
@@ -4490,7 +4500,7 @@
       </c>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="11" t="s">
         <v>18</v>
@@ -4508,7 +4518,7 @@
       </c>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="11" t="s">
         <v>19</v>
@@ -4526,7 +4536,7 @@
       </c>
       <c r="H10" s="11"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="11" t="s">
         <v>20</v>
@@ -4544,7 +4554,7 @@
       </c>
       <c r="H11" s="11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="11" t="s">
         <v>23</v>
@@ -4562,7 +4572,7 @@
       </c>
       <c r="H12" s="11"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="11" t="s">
         <v>26</v>
@@ -4580,7 +4590,7 @@
       </c>
       <c r="H13" s="11"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="11" t="s">
         <v>31</v>
@@ -4598,7 +4608,7 @@
       </c>
       <c r="H14" s="11"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -4608,7 +4618,7 @@
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -4631,32 +4641,32 @@
       <selection activeCell="D38" sqref="B36:D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" style="5" customWidth="1"/>
-    <col min="3" max="4" width="8.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" style="23" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="4.44140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" style="5" customWidth="1"/>
+    <col min="3" max="4" width="8.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" style="23" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="11"/>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
       <c r="E1" s="21"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="25"/>
+      <c r="D2" s="28"/>
       <c r="E2" s="21"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="8" t="s">
         <v>0</v>
@@ -4672,7 +4682,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="11" t="s">
         <v>9</v>
@@ -4685,7 +4695,7 @@
       </c>
       <c r="E4" s="22"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="11" t="s">
         <v>10</v>
@@ -4698,7 +4708,7 @@
       </c>
       <c r="E5" s="22"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="11" t="s">
         <v>14</v>
@@ -4711,7 +4721,7 @@
       </c>
       <c r="E6" s="22"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="11" t="s">
         <v>19</v>
@@ -4724,7 +4734,7 @@
       </c>
       <c r="E7" s="22"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="11" t="s">
         <v>20</v>
@@ -4737,7 +4747,7 @@
       </c>
       <c r="E8" s="22"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="11" t="s">
         <v>23</v>
@@ -4750,7 +4760,7 @@
       </c>
       <c r="E9" s="22"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="11" t="s">
         <v>31</v>
@@ -4763,7 +4773,7 @@
       </c>
       <c r="E10" s="22"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="11" t="s">
         <v>36</v>
@@ -4776,23 +4786,23 @@
       </c>
       <c r="E11" s="22"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="21"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="D13" s="25"/>
+      <c r="D13" s="28"/>
       <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="8" t="s">
         <v>0</v>
@@ -4805,7 +4815,7 @@
       </c>
       <c r="E14" s="22"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="11" t="s">
         <v>10</v>
@@ -4818,7 +4828,7 @@
       </c>
       <c r="E15" s="22"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="11" t="s">
         <v>14</v>
@@ -4831,7 +4841,7 @@
       </c>
       <c r="E16" s="22"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="11" t="s">
         <v>18</v>
@@ -4844,7 +4854,7 @@
       </c>
       <c r="E17" s="22"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="11" t="s">
         <v>19</v>
@@ -4857,7 +4867,7 @@
       </c>
       <c r="E18" s="22"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
       <c r="B19" s="11" t="s">
         <v>31</v>
@@ -4870,23 +4880,23 @@
       </c>
       <c r="E19" s="22"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="14"/>
       <c r="D20" s="20"/>
       <c r="E20" s="22"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="D21" s="25"/>
+      <c r="D21" s="28"/>
       <c r="E21" s="21"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
       <c r="B22" s="8" t="s">
         <v>0</v>
@@ -4899,7 +4909,7 @@
       </c>
       <c r="E22" s="22"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>
       <c r="B23" s="11" t="s">
         <v>8</v>
@@ -4912,7 +4922,7 @@
       </c>
       <c r="E23" s="22"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
       <c r="B24" s="11" t="s">
         <v>14</v>
@@ -4925,7 +4935,7 @@
       </c>
       <c r="E24" s="22"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" s="11" t="s">
         <v>16</v>
@@ -4938,7 +4948,7 @@
       </c>
       <c r="E25" s="22"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
       <c r="B26" s="11" t="s">
         <v>18</v>
@@ -4951,7 +4961,7 @@
       </c>
       <c r="E26" s="22"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
       <c r="B27" s="11" t="s">
         <v>20</v>
@@ -4964,7 +4974,7 @@
       </c>
       <c r="E27" s="22"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
       <c r="B28" s="11" t="s">
         <v>23</v>
@@ -4977,7 +4987,7 @@
       </c>
       <c r="E28" s="22"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="11"/>
       <c r="B29" s="11" t="s">
         <v>26</v>
@@ -4990,7 +5000,7 @@
       </c>
       <c r="E29" s="22"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="11"/>
       <c r="B30" s="11" t="s">
         <v>30</v>
@@ -5003,7 +5013,7 @@
       </c>
       <c r="E30" s="22"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="11"/>
       <c r="B31" s="11" t="s">
         <v>31</v>
@@ -5016,23 +5026,23 @@
       </c>
       <c r="E31" s="22"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="11"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
       <c r="E32" s="22"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
-      <c r="C33" s="25" t="s">
+      <c r="C33" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="D33" s="25"/>
+      <c r="D33" s="28"/>
       <c r="E33" s="22"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="11"/>
       <c r="B34" s="8" t="s">
         <v>0</v>
@@ -5045,7 +5055,7 @@
       </c>
       <c r="E34" s="22"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="11"/>
       <c r="B35" s="11" t="s">
         <v>10</v>
@@ -5058,7 +5068,7 @@
       </c>
       <c r="E35" s="22"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="11"/>
       <c r="B36" s="11" t="s">
         <v>18</v>
@@ -5071,7 +5081,7 @@
       </c>
       <c r="E36" s="22"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="11"/>
       <c r="B37" s="11" t="s">
         <v>26</v>
@@ -5084,7 +5094,7 @@
       </c>
       <c r="E37" s="22"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="11"/>
       <c r="B38" s="11" t="s">
         <v>31</v>
@@ -5097,7 +5107,7 @@
       </c>
       <c r="E38" s="22"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>

</xml_diff>

<commit_message>
Updated draft to committee Addressed TS review comments Table updated
</commit_message>
<xml_diff>
--- a/Ch1_Tables.xlsx
+++ b/Ch1_Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtpriest\Desktop\GradSchool\Thesis2019_Ch1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BC230F-8AF4-481D-A02B-6E77F9CC32D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C74C86F-0D28-47F9-8929-C4500E6236AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EC0383BB-9F3C-437D-BF2A-12F22EF652FA}"/>
   </bookViews>
@@ -27,7 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="124">
   <si>
     <t>Species</t>
   </si>
@@ -404,6 +406,9 @@
   </si>
   <si>
     <t>replaced 0 with &lt;0.001</t>
+  </si>
+  <si>
+    <t>Slope</t>
   </si>
 </sst>
 </file>
@@ -3631,7 +3636,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3693,28 +3698,28 @@
         <v>0</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>116</v>
       </c>
       <c r="E3" s="18"/>
       <c r="F3" s="18" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="G3" s="18" t="s">
         <v>116</v>
       </c>
       <c r="H3" s="18"/>
       <c r="I3" s="18" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>116</v>
       </c>
       <c r="K3" s="11"/>
       <c r="L3" s="18" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="M3" s="18" t="s">
         <v>116</v>

</xml_diff>

<commit_message>
Updated many minor fixes
</commit_message>
<xml_diff>
--- a/Ch1_Tables.xlsx
+++ b/Ch1_Tables.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtpriest\Desktop\GradSchool\Thesis2019_Ch1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C74C86F-0D28-47F9-8929-C4500E6236AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5CBCB7-46DE-4C0A-8FEB-38B3EAD1CE92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EC0383BB-9F3C-437D-BF2A-12F22EF652FA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{EC0383BB-9F3C-437D-BF2A-12F22EF652FA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Table1" sheetId="1" r:id="rId1"/>
-    <sheet name="TopSppCalc" sheetId="2" r:id="rId2"/>
-    <sheet name="Table2" sheetId="3" r:id="rId3"/>
+    <sheet name="CH1_Table1_final" sheetId="1" r:id="rId1"/>
+    <sheet name="CH1_Table2_final" sheetId="3" r:id="rId2"/>
+    <sheet name="TopSppCalc" sheetId="2" r:id="rId3"/>
     <sheet name="Table2_V2" sheetId="4" r:id="rId4"/>
     <sheet name="Table2_V3" sheetId="5" r:id="rId5"/>
   </sheets>
@@ -506,7 +506,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -566,6 +566,51 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -881,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA1E8B1-AAD0-407A-9308-23B107A875A9}">
-  <dimension ref="A1:O76"/>
+  <dimension ref="A1:O77"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView topLeftCell="F16" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -898,950 +943,935 @@
     <col min="14" max="14" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H1" s="46"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="46"/>
+    </row>
+    <row r="2" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="8" t="s">
+      <c r="H2" s="46"/>
+      <c r="I2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N2" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="O1" s="7"/>
-    </row>
-    <row r="2" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="O2" s="47"/>
+    </row>
+    <row r="3" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="F3">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="11" t="str">
-        <f>A2&amp;G2</f>
+      <c r="H3" s="46"/>
+      <c r="I3" s="11" t="str">
+        <f>A3&amp;G3</f>
         <v>Arctic Char†</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J3" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="13">
-        <f>B2</f>
+      <c r="K3" s="13">
+        <f>B3</f>
         <v>1</v>
       </c>
-      <c r="L2" s="14">
-        <f>C2</f>
-        <v>0</v>
-      </c>
-      <c r="M2" s="15" t="s">
+      <c r="L3" s="14">
+        <f>C3</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="N2" s="16">
-        <f>F2</f>
+      <c r="N3" s="16">
+        <f>F3</f>
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="O2" s="7"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1">
-        <v>251131</v>
-      </c>
-      <c r="C3" s="2">
-        <v>897</v>
-      </c>
-      <c r="D3">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1">
-        <v>10760</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="4"/>
-      <c r="I3" s="11" t="str">
-        <f t="shared" ref="I3:I32" si="0">A3&amp;G3</f>
-        <v>Arctic Cisco</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" s="13">
-        <f t="shared" ref="K3:K32" si="1">B3</f>
-        <v>251131</v>
-      </c>
-      <c r="L3" s="14">
-        <f t="shared" ref="L3:L32" si="2">C3</f>
-        <v>897</v>
-      </c>
-      <c r="M3" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="N3" s="16">
-        <f t="shared" ref="N3:N32" si="3">F3</f>
-        <v>1</v>
-      </c>
-      <c r="O3" s="7"/>
+      <c r="O3" s="47"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
+        <v>251131</v>
+      </c>
+      <c r="C4" s="2">
+        <v>897</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1">
+        <v>10760</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="11" t="str">
+        <f t="shared" ref="I4:I33" si="0">A4&amp;G4</f>
+        <v>Arctic Cisco</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="13">
+        <f t="shared" ref="K4:K33" si="1">B4</f>
+        <v>251131</v>
+      </c>
+      <c r="L4" s="14">
+        <f t="shared" ref="L4:L33" si="2">C4</f>
+        <v>897</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="N4" s="16">
+        <f t="shared" ref="N4:N33" si="3">F4</f>
+        <v>1</v>
+      </c>
+      <c r="O4" s="47"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="1">
         <v>595271</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C5" s="2">
         <v>2126</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
         <v>180483</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>0.89600000000000002</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="I4" s="11" t="str">
+      <c r="G5" s="4"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Arctic Cod</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J5" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K5" s="13">
         <f t="shared" si="1"/>
         <v>595271</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L5" s="14">
         <f t="shared" si="2"/>
         <v>2126</v>
       </c>
-      <c r="M4" s="15" t="s">
+      <c r="M5" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="N4" s="16">
+      <c r="N5" s="16">
         <f t="shared" si="3"/>
         <v>0.89600000000000002</v>
       </c>
-      <c r="O4" s="7"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="O5" s="47"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="1">
         <v>182323</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C6" s="2">
         <v>651</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>10</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E6" s="1">
         <v>3297</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>1</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="I5" s="11" t="str">
+      <c r="G6" s="4"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Arctic Flounder</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J6" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K6" s="13">
         <f t="shared" si="1"/>
         <v>182323</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L6" s="14">
         <f t="shared" si="2"/>
         <v>651</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="M6" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="N5" s="16">
+      <c r="N6" s="16">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="O5" s="7"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="O6" s="47"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>845</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>3</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
         <v>141</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>0.46400000000000002</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="I6" s="11" t="str">
+      <c r="G7" s="4"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Arctic Grayling</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J7" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K7" s="13">
         <f t="shared" si="1"/>
         <v>845</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L7" s="14">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="M6" s="15" t="s">
+      <c r="M7" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="N6" s="16">
+      <c r="N7" s="16">
         <f t="shared" si="3"/>
         <v>0.46400000000000002</v>
       </c>
-      <c r="O6" s="7"/>
-    </row>
-    <row r="7" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="O7" s="47"/>
+    </row>
+    <row r="8" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>53</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
         <v>10</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>0.1</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="11" t="str">
+      <c r="H8" s="46"/>
+      <c r="I8" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Bering Cisco†</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J8" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K8" s="13">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L8" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M7" s="15" t="s">
+      <c r="M8" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="N7" s="16">
+      <c r="N8" s="16">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="O7" s="7"/>
-    </row>
-    <row r="8" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="O8" s="47"/>
+    </row>
+    <row r="9" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>3</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
         <v>1</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="11" t="str">
+      <c r="H9" s="46"/>
+      <c r="I9" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Bering Wolffish†</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J9" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K9" s="13">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L9" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M8" s="15" t="s">
+      <c r="M9" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="N8" s="16">
+      <c r="N9" s="16">
         <f t="shared" si="3"/>
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="O8" s="7"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="O9" s="47"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B10" s="1">
         <v>172310</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C10" s="2">
         <v>615</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>5</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E10" s="1">
         <v>5858</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <v>1</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="I9" s="11" t="str">
+      <c r="G10" s="4"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Broad Whitefish</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J10" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="K9" s="13">
+      <c r="K10" s="13">
         <f t="shared" si="1"/>
         <v>172310</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L10" s="14">
         <f t="shared" si="2"/>
         <v>615</v>
       </c>
-      <c r="M9" s="15" t="s">
+      <c r="M10" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="N9" s="16">
+      <c r="N10" s="16">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="O9" s="7"/>
-    </row>
-    <row r="10" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="O10" s="47"/>
+    </row>
+    <row r="11" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>19</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
         <v>3</v>
       </c>
-      <c r="F10">
+      <c r="F11">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="11" t="str">
+      <c r="H11" s="46"/>
+      <c r="I11" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Burbot†</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J11" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K11" s="13">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="L10" s="14">
+      <c r="L11" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M10" s="15" t="s">
+      <c r="M11" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="N10" s="16">
+      <c r="N11" s="16">
         <f t="shared" si="3"/>
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="O10" s="7"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="O11" s="47"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>950</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>3</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
         <v>262</v>
       </c>
-      <c r="F11">
+      <c r="F12">
         <v>0.311</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="I11" s="11" t="str">
+      <c r="G12" s="4"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Capelin</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J12" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="K11" s="13">
+      <c r="K12" s="13">
         <f t="shared" si="1"/>
         <v>950</v>
       </c>
-      <c r="L11" s="14">
+      <c r="L12" s="14">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M12" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="N11" s="16">
+      <c r="N12" s="16">
         <f t="shared" si="3"/>
         <v>0.311</v>
       </c>
-      <c r="O11" s="7"/>
-    </row>
-    <row r="12" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="O12" s="47"/>
+    </row>
+    <row r="13" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>32</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
         <v>3</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="11" t="str">
+      <c r="H13" s="46"/>
+      <c r="I13" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Chum Salmon†</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="J13" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K13" s="13">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="L12" s="14">
+      <c r="L13" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M12" s="15" t="s">
+      <c r="M13" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="N12" s="16">
+      <c r="N13" s="16">
         <f t="shared" si="3"/>
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="O12" s="7"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="O13" s="47"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B14" s="1">
         <v>32055</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>114</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1">
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
         <v>1068</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <v>0.98899999999999999</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="I13" s="11" t="str">
+      <c r="G14" s="4"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Dolly Varden</v>
       </c>
-      <c r="J13" s="12" t="s">
+      <c r="J14" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="K13" s="13">
+      <c r="K14" s="13">
         <f t="shared" si="1"/>
         <v>32055</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L14" s="14">
         <f t="shared" si="2"/>
         <v>114</v>
       </c>
-      <c r="M13" s="15" t="s">
+      <c r="M14" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="N13" s="16">
+      <c r="N14" s="16">
         <f t="shared" si="3"/>
         <v>0.98899999999999999</v>
       </c>
-      <c r="O13" s="7"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="O14" s="47"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B15" s="1">
         <v>139952</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C15" s="2">
         <v>500</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <v>10</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E15" s="1">
         <v>2482</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <v>1</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="I14" s="11" t="str">
+      <c r="G15" s="4"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Fourhorn Sculpin</v>
       </c>
-      <c r="J14" s="12" t="s">
+      <c r="J15" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="K14" s="13">
+      <c r="K15" s="13">
         <f t="shared" si="1"/>
         <v>139952</v>
       </c>
-      <c r="L14" s="14">
+      <c r="L15" s="14">
         <f t="shared" si="2"/>
         <v>500</v>
       </c>
-      <c r="M14" s="15" t="s">
+      <c r="M15" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="N14" s="16">
+      <c r="N15" s="16">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="O14" s="7"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="O15" s="47"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B16" s="1">
         <v>32575</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>116</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1">
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
         <v>865</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>0.97899999999999998</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="I15" s="11" t="str">
+      <c r="G16" s="4"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Humpback Whitefish</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="J16" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="K15" s="13">
+      <c r="K16" s="13">
         <f t="shared" si="1"/>
         <v>32575</v>
       </c>
-      <c r="L15" s="14">
+      <c r="L16" s="14">
         <f t="shared" si="2"/>
         <v>116</v>
       </c>
-      <c r="M15" s="15" t="s">
+      <c r="M16" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="N15" s="16">
+      <c r="N16" s="16">
         <f t="shared" si="3"/>
         <v>0.97899999999999998</v>
       </c>
-      <c r="O15" s="7"/>
-    </row>
-    <row r="16" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="O16" s="47"/>
+    </row>
+    <row r="17" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>2</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
         <v>2</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="11" t="str">
+      <c r="H17" s="46"/>
+      <c r="I17" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Kelp Greenling†</v>
       </c>
-      <c r="J16" s="12" t="s">
+      <c r="J17" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="K16" s="13">
+      <c r="K17" s="13">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="L16" s="14">
+      <c r="L17" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M16" s="15" t="s">
+      <c r="M17" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="N16" s="16">
+      <c r="N17" s="16">
         <f t="shared" si="3"/>
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="O16" s="7"/>
-    </row>
-    <row r="17" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="O17" s="47"/>
+    </row>
+    <row r="18" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>4</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
         <v>2</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I17" s="11" t="str">
+      <c r="H18" s="46"/>
+      <c r="I18" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Kelp Snailfish†</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="J18" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="K17" s="13">
+      <c r="K18" s="13">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="L17" s="14">
+      <c r="L18" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M17" s="15" t="s">
+      <c r="M18" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="N17" s="16">
+      <c r="N18" s="16">
         <f t="shared" si="3"/>
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="O17" s="7"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="O18" s="47"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B19" s="1">
         <v>231000</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C19" s="2">
         <v>825</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <v>12</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E19" s="1">
         <v>4327</v>
       </c>
-      <c r="F18">
+      <c r="F19">
         <v>1</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="I18" s="11" t="str">
+      <c r="G19" s="4"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Least Cisco</v>
       </c>
-      <c r="J18" s="12" t="s">
+      <c r="J19" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="K18" s="13">
+      <c r="K19" s="13">
         <f t="shared" si="1"/>
         <v>231000</v>
       </c>
-      <c r="L18" s="14">
+      <c r="L19" s="14">
         <f t="shared" si="2"/>
         <v>825</v>
       </c>
-      <c r="M18" s="15" t="s">
+      <c r="M19" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="N18" s="16">
+      <c r="N19" s="16">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="O18" s="7"/>
-    </row>
-    <row r="19" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="O19" s="47"/>
+    </row>
+    <row r="20" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>1</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
         <v>1</v>
       </c>
-      <c r="F19">
+      <c r="F20">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I19" s="11" t="str">
+      <c r="H20" s="46"/>
+      <c r="I20" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Longnose Sucker†</v>
       </c>
-      <c r="J19" s="12" t="s">
+      <c r="J20" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="K19" s="13">
+      <c r="K20" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L19" s="14">
+      <c r="L20" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M19" s="15" t="s">
+      <c r="M20" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="N19" s="16">
+      <c r="N20" s="16">
         <f t="shared" si="3"/>
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="O19" s="7"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="O20" s="47"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B21" s="1">
         <v>8983</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>32</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20" s="1">
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
         <v>909</v>
       </c>
-      <c r="F20">
+      <c r="F21">
         <v>0.754</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="I20" s="11" t="str">
+      <c r="G21" s="4"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Ninespine Stickleback</v>
       </c>
-      <c r="J20" s="12" t="s">
+      <c r="J21" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="K20" s="13">
+      <c r="K21" s="13">
         <f t="shared" si="1"/>
         <v>8983</v>
       </c>
-      <c r="L20" s="14">
+      <c r="L21" s="14">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="M20" s="15" t="s">
+      <c r="M21" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="N20" s="16">
+      <c r="N21" s="16">
         <f t="shared" si="3"/>
         <v>0.754</v>
       </c>
-      <c r="O20" s="7"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21">
-        <v>487</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>40</v>
-      </c>
-      <c r="F21">
-        <v>0.34599999999999997</v>
-      </c>
-      <c r="G21" s="4"/>
-      <c r="I21" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>Pacific Herring</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="K21" s="13">
-        <f t="shared" si="1"/>
-        <v>487</v>
-      </c>
-      <c r="L21" s="14">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="M21" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="N21" s="16">
-        <f t="shared" si="3"/>
-        <v>0.34599999999999997</v>
-      </c>
-      <c r="O21" s="7"/>
+      <c r="O21" s="47"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22">
-        <v>530</v>
+        <v>487</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -1850,263 +1880,267 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="F22">
-        <v>0.36099999999999999</v>
+        <v>0.34599999999999997</v>
       </c>
       <c r="G22" s="4"/>
+      <c r="H22" s="46"/>
       <c r="I22" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Pink Salmon</v>
+        <v>Pacific Herring</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K22" s="13">
         <f t="shared" si="1"/>
-        <v>530</v>
+        <v>487</v>
       </c>
       <c r="L22" s="14">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="M22" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N22" s="16">
         <f t="shared" si="3"/>
-        <v>0.36099999999999999</v>
-      </c>
-      <c r="O22" s="7"/>
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="O22" s="47"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="1">
-        <v>77433</v>
-      </c>
-      <c r="C23" s="2">
-        <v>277</v>
+        <v>27</v>
+      </c>
+      <c r="B23">
+        <v>530</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
       </c>
       <c r="D23">
-        <v>4</v>
-      </c>
-      <c r="E23" s="1">
-        <v>2335</v>
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>72</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>0.36099999999999999</v>
       </c>
       <c r="G23" s="4"/>
+      <c r="H23" s="46"/>
       <c r="I23" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Rainbow Smelt</v>
+        <v>Pink Salmon</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K23" s="13">
         <f t="shared" si="1"/>
-        <v>77433</v>
+        <v>530</v>
       </c>
       <c r="L23" s="14">
         <f t="shared" si="2"/>
-        <v>277</v>
+        <v>2</v>
       </c>
       <c r="M23" s="15" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="N23" s="16">
         <f t="shared" si="3"/>
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="O23" s="47"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="1">
+        <v>77433</v>
+      </c>
+      <c r="C24" s="2">
+        <v>277</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2335</v>
+      </c>
+      <c r="F24">
         <v>1</v>
       </c>
-      <c r="O23" s="7"/>
-    </row>
-    <row r="24" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24">
-        <v>9</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>4</v>
-      </c>
-      <c r="F24">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="46"/>
       <c r="I24" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Rock Greenling†</v>
+        <v>Rainbow Smelt</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K24" s="13">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>77433</v>
       </c>
       <c r="L24" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>277</v>
       </c>
       <c r="M24" s="15" t="s">
-        <v>77</v>
+        <v>111</v>
       </c>
       <c r="N24" s="16">
         <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O24" s="47"/>
+    </row>
+    <row r="25" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25">
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+      <c r="F25">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="O24" s="7"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="1">
-        <v>7318</v>
-      </c>
-      <c r="C25">
-        <v>26</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>380</v>
-      </c>
-      <c r="F25">
-        <v>0.68600000000000005</v>
-      </c>
-      <c r="G25" s="4"/>
+      <c r="G25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25" s="46"/>
       <c r="I25" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Round Whitefish</v>
+        <v>Rock Greenling†</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K25" s="13">
         <f t="shared" si="1"/>
-        <v>7318</v>
+        <v>9</v>
       </c>
       <c r="L25" s="14">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="M25" s="15" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="N25" s="16">
         <f t="shared" si="3"/>
-        <v>0.68600000000000005</v>
-      </c>
-      <c r="O25" s="7"/>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="O25" s="47"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="1">
-        <v>50716</v>
+        <v>7318</v>
       </c>
       <c r="C26">
-        <v>181</v>
+        <v>26</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
-      <c r="E26" s="1">
-        <v>2866</v>
+      <c r="E26">
+        <v>380</v>
       </c>
       <c r="F26">
-        <v>0.96799999999999997</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="G26" s="4"/>
+      <c r="H26" s="46"/>
       <c r="I26" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Saffron Cod</v>
+        <v>Round Whitefish</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K26" s="13">
         <f t="shared" si="1"/>
-        <v>50716</v>
+        <v>7318</v>
       </c>
       <c r="L26" s="14">
         <f t="shared" si="2"/>
-        <v>181</v>
+        <v>26</v>
       </c>
       <c r="M26" s="15" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="N26" s="16">
         <f t="shared" si="3"/>
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="O26" s="47"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="1">
+        <v>50716</v>
+      </c>
+      <c r="C27">
+        <v>181</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>2866</v>
+      </c>
+      <c r="F27">
         <v>0.96799999999999997</v>
       </c>
-      <c r="O26" s="7"/>
-    </row>
-    <row r="27" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="46"/>
       <c r="I27" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Shorthorn Sculpin†</v>
-      </c>
-      <c r="J27" s="17" t="s">
-        <v>64</v>
+        <v>Saffron Cod</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="K27" s="13">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>50716</v>
       </c>
       <c r="L27" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>181</v>
       </c>
       <c r="M27" s="15" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="N27" s="16">
         <f t="shared" si="3"/>
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="O27" s="7"/>
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="O27" s="47"/>
     </row>
     <row r="28" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -2126,12 +2160,13 @@
       <c r="G28" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="H28" s="46"/>
       <c r="I28" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Slender Eelblenny†</v>
-      </c>
-      <c r="J28" s="12" t="s">
-        <v>65</v>
+        <v>Shorthorn Sculpin†</v>
+      </c>
+      <c r="J28" s="17" t="s">
+        <v>64</v>
       </c>
       <c r="K28" s="13">
         <f t="shared" si="1"/>
@@ -2148,14 +2183,14 @@
         <f t="shared" si="3"/>
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="O28" s="7"/>
+      <c r="O28" s="47"/>
     </row>
     <row r="29" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -2164,44 +2199,45 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29">
-        <v>1.7999999999999999E-2</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="H29" s="46"/>
       <c r="I29" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Slimy Sculpin†</v>
+        <v>Slender Eelblenny†</v>
       </c>
       <c r="J29" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K29" s="13">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L29" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M29" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N29" s="16">
         <f t="shared" si="3"/>
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="O29" s="7"/>
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="O29" s="47"/>
     </row>
     <row r="30" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -2210,291 +2246,327 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F30">
-        <v>4.0000000000000001E-3</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="H30" s="46"/>
       <c r="I30" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Sockeye Salmon†</v>
+        <v>Slimy Sculpin†</v>
       </c>
       <c r="J30" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K30" s="13">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L30" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M30" s="15" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N30" s="16">
         <f t="shared" si="3"/>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="O30" s="47"/>
+    </row>
+    <row r="31" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="O30" s="7"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31">
-        <v>577</v>
-      </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>48</v>
-      </c>
-      <c r="F31">
-        <v>0.36099999999999999</v>
-      </c>
-      <c r="G31" s="4"/>
+      <c r="G31" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H31" s="46"/>
       <c r="I31" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Threespine Stickleback</v>
+        <v>Sockeye Salmon†</v>
       </c>
       <c r="J31" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K31" s="13">
         <f t="shared" si="1"/>
-        <v>577</v>
+        <v>1</v>
       </c>
       <c r="L31" s="14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M31" s="15" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="N31" s="16">
         <f t="shared" si="3"/>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="O31" s="47"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32">
+        <v>577</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>48</v>
+      </c>
+      <c r="F32">
         <v>0.36099999999999999</v>
       </c>
-      <c r="O31" s="7"/>
-    </row>
-    <row r="32" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="G32" s="4"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>Threespine Stickleback</v>
+      </c>
+      <c r="J32" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="K32" s="41">
+        <f t="shared" si="1"/>
+        <v>577</v>
+      </c>
+      <c r="L32" s="30">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M32" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="N32" s="42">
+        <f t="shared" si="3"/>
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="O32" s="47"/>
+    </row>
+    <row r="33" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>37</v>
       </c>
-      <c r="B32">
+      <c r="B33">
         <v>2</v>
       </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
         <v>2</v>
       </c>
-      <c r="F32">
+      <c r="F33">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G33" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I32" s="11" t="str">
+      <c r="H33" s="46"/>
+      <c r="I33" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Whitespotted Greenling†</v>
       </c>
-      <c r="J32" s="12" t="s">
+      <c r="J33" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="K32" s="13">
+      <c r="K33" s="44">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="L32" s="14">
+      <c r="L33" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M32" s="15" t="s">
+      <c r="M33" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="N32" s="16">
+      <c r="N33" s="45">
         <f t="shared" si="3"/>
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="O32" s="7"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="N33" s="7"/>
-      <c r="O33" s="7"/>
+      <c r="O33" s="47"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="N34" s="7"/>
-      <c r="O34" s="7"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K36" s="6">
-        <f>SUM(K2:K32)</f>
+      <c r="H34" s="46"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="47"/>
+      <c r="O34" s="47"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K37" s="6">
+        <f>SUM(K3:K33)</f>
         <v>1784593</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>0</v>
-      </c>
-      <c r="B45" t="s">
-        <v>1</v>
-      </c>
-      <c r="C45" t="s">
-        <v>2</v>
-      </c>
-      <c r="D45" t="s">
-        <v>3</v>
-      </c>
-      <c r="E45" t="s">
-        <v>4</v>
-      </c>
-      <c r="F45" t="s">
-        <v>5</v>
-      </c>
-      <c r="G45" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>7</v>
-      </c>
-      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="B46" t="s">
         <v>1</v>
       </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-      <c r="F46">
-        <v>4.0000000000000001E-3</v>
+      <c r="C46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46" t="s">
+        <v>5</v>
+      </c>
+      <c r="G46" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>8</v>
-      </c>
-      <c r="B47" s="1">
-        <v>251131</v>
+        <v>7</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
       </c>
       <c r="C47">
-        <v>897</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>15</v>
-      </c>
-      <c r="E47" s="1">
-        <v>10760</v>
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
       </c>
       <c r="F47">
-        <v>1</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B48" s="1">
-        <v>595271</v>
-      </c>
-      <c r="C48" s="1">
-        <v>2126</v>
+        <v>251131</v>
+      </c>
+      <c r="C48">
+        <v>897</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E48" s="1">
-        <v>180483</v>
+        <v>10760</v>
       </c>
       <c r="F48">
-        <v>0.89600000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B49" s="1">
-        <v>182323</v>
-      </c>
-      <c r="C49">
-        <v>651</v>
+        <v>595271</v>
+      </c>
+      <c r="C49" s="1">
+        <v>2126</v>
       </c>
       <c r="D49">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E49" s="1">
-        <v>3297</v>
+        <v>180483</v>
       </c>
       <c r="F49">
-        <v>1</v>
+        <v>0.89600000000000002</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>11</v>
-      </c>
-      <c r="B50">
-        <v>845</v>
+        <v>10</v>
+      </c>
+      <c r="B50" s="1">
+        <v>182323</v>
       </c>
       <c r="C50">
-        <v>3</v>
+        <v>651</v>
       </c>
       <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="E50">
-        <v>141</v>
+        <v>10</v>
+      </c>
+      <c r="E50" s="1">
+        <v>3297</v>
       </c>
       <c r="F50">
-        <v>0.46400000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B51">
-        <v>53</v>
+        <v>845</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D51">
         <v>0</v>
       </c>
       <c r="E51">
-        <v>10</v>
+        <v>141</v>
       </c>
       <c r="F51">
-        <v>0.1</v>
+        <v>0.46400000000000002</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B52">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -2503,178 +2575,178 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52">
-        <v>1.0999999999999999E-2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>14</v>
-      </c>
-      <c r="B53" s="1">
-        <v>172310</v>
+        <v>13</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
       </c>
       <c r="C53">
-        <v>615</v>
+        <v>0</v>
       </c>
       <c r="D53">
-        <v>5</v>
-      </c>
-      <c r="E53" s="1">
-        <v>5858</v>
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
       </c>
       <c r="F53">
-        <v>1</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>15</v>
-      </c>
-      <c r="B54">
-        <v>19</v>
+        <v>14</v>
+      </c>
+      <c r="B54" s="1">
+        <v>172310</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>615</v>
       </c>
       <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="E54" s="1">
+        <v>5858</v>
       </c>
       <c r="F54">
-        <v>4.5999999999999999E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B55">
-        <v>950</v>
+        <v>19</v>
       </c>
       <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
         <v>3</v>
       </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-      <c r="E55">
-        <v>262</v>
-      </c>
       <c r="F55">
-        <v>0.311</v>
+        <v>4.5999999999999999E-2</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B56">
-        <v>32</v>
+        <v>950</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D56">
         <v>0</v>
       </c>
       <c r="E56">
-        <v>3</v>
+        <v>262</v>
       </c>
       <c r="F56">
-        <v>9.2999999999999999E-2</v>
+        <v>0.311</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>18</v>
-      </c>
-      <c r="B57" s="1">
-        <v>32055</v>
+        <v>17</v>
+      </c>
+      <c r="B57">
+        <v>32</v>
       </c>
       <c r="C57">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="D57">
         <v>0</v>
       </c>
-      <c r="E57" s="1">
-        <v>1068</v>
+      <c r="E57">
+        <v>3</v>
       </c>
       <c r="F57">
-        <v>0.98899999999999999</v>
+        <v>9.2999999999999999E-2</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B58" s="1">
-        <v>139952</v>
+        <v>32055</v>
       </c>
       <c r="C58">
-        <v>500</v>
+        <v>114</v>
       </c>
       <c r="D58">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E58" s="1">
-        <v>2482</v>
+        <v>1068</v>
       </c>
       <c r="F58">
-        <v>1</v>
+        <v>0.98899999999999999</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B59" s="1">
-        <v>32575</v>
+        <v>139952</v>
       </c>
       <c r="C59">
-        <v>116</v>
+        <v>500</v>
       </c>
       <c r="D59">
-        <v>0</v>
-      </c>
-      <c r="E59">
-        <v>865</v>
+        <v>10</v>
+      </c>
+      <c r="E59" s="1">
+        <v>2482</v>
       </c>
       <c r="F59">
-        <v>0.97899999999999998</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>21</v>
-      </c>
-      <c r="B60">
-        <v>2</v>
+        <v>20</v>
+      </c>
+      <c r="B60" s="1">
+        <v>32575</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="D60">
         <v>0</v>
       </c>
       <c r="E60">
-        <v>2</v>
+        <v>865</v>
       </c>
       <c r="F60">
-        <v>4.0000000000000001E-3</v>
+        <v>0.97899999999999998</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B61">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -2686,95 +2758,95 @@
         <v>2</v>
       </c>
       <c r="F61">
-        <v>7.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>23</v>
-      </c>
-      <c r="B62" s="1">
-        <v>231000</v>
+        <v>22</v>
+      </c>
+      <c r="B62">
+        <v>4</v>
       </c>
       <c r="C62">
-        <v>825</v>
+        <v>0</v>
       </c>
       <c r="D62">
-        <v>12</v>
-      </c>
-      <c r="E62" s="1">
-        <v>4327</v>
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>2</v>
       </c>
       <c r="F62">
-        <v>1</v>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>24</v>
-      </c>
-      <c r="B63">
+        <v>23</v>
+      </c>
+      <c r="B63" s="1">
+        <v>231000</v>
+      </c>
+      <c r="C63">
+        <v>825</v>
+      </c>
+      <c r="D63">
+        <v>12</v>
+      </c>
+      <c r="E63" s="1">
+        <v>4327</v>
+      </c>
+      <c r="F63">
         <v>1</v>
-      </c>
-      <c r="C63">
-        <v>0</v>
-      </c>
-      <c r="D63">
-        <v>0</v>
-      </c>
-      <c r="E63">
-        <v>1</v>
-      </c>
-      <c r="F63">
-        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>25</v>
-      </c>
-      <c r="B64" s="1">
-        <v>8983</v>
+        <v>24</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
       </c>
       <c r="C64">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="D64">
         <v>0</v>
       </c>
       <c r="E64">
-        <v>909</v>
+        <v>1</v>
       </c>
       <c r="F64">
-        <v>0.754</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>26</v>
-      </c>
-      <c r="B65">
-        <v>487</v>
+        <v>25</v>
+      </c>
+      <c r="B65" s="1">
+        <v>8983</v>
       </c>
       <c r="C65">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D65">
         <v>0</v>
       </c>
       <c r="E65">
-        <v>40</v>
+        <v>909</v>
       </c>
       <c r="F65">
-        <v>0.34599999999999997</v>
+        <v>0.754</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B66">
-        <v>530</v>
+        <v>487</v>
       </c>
       <c r="C66">
         <v>2</v>
@@ -2783,115 +2855,115 @@
         <v>0</v>
       </c>
       <c r="E66">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="F66">
-        <v>0.36099999999999999</v>
+        <v>0.34599999999999997</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>28</v>
-      </c>
-      <c r="B67" s="1">
-        <v>77433</v>
+        <v>27</v>
+      </c>
+      <c r="B67">
+        <v>530</v>
       </c>
       <c r="C67">
-        <v>277</v>
+        <v>2</v>
       </c>
       <c r="D67">
-        <v>4</v>
-      </c>
-      <c r="E67" s="1">
-        <v>2335</v>
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>72</v>
       </c>
       <c r="F67">
-        <v>1</v>
+        <v>0.36099999999999999</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>29</v>
-      </c>
-      <c r="B68">
-        <v>9</v>
+        <v>28</v>
+      </c>
+      <c r="B68" s="1">
+        <v>77433</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>277</v>
       </c>
       <c r="D68">
-        <v>0</v>
-      </c>
-      <c r="E68">
         <v>4</v>
       </c>
+      <c r="E68" s="1">
+        <v>2335</v>
+      </c>
       <c r="F68">
-        <v>1.7999999999999999E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>30</v>
-      </c>
-      <c r="B69" s="1">
-        <v>7318</v>
+        <v>29</v>
+      </c>
+      <c r="B69">
+        <v>9</v>
       </c>
       <c r="C69">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D69">
         <v>0</v>
       </c>
       <c r="E69">
-        <v>380</v>
+        <v>4</v>
       </c>
       <c r="F69">
-        <v>0.68600000000000005</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B70" s="1">
-        <v>50716</v>
+        <v>7318</v>
       </c>
       <c r="C70">
-        <v>181</v>
+        <v>26</v>
       </c>
       <c r="D70">
         <v>0</v>
       </c>
-      <c r="E70" s="1">
-        <v>2866</v>
+      <c r="E70">
+        <v>380</v>
       </c>
       <c r="F70">
-        <v>0.96799999999999997</v>
+        <v>0.68600000000000005</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>32</v>
-      </c>
-      <c r="B71">
-        <v>2</v>
+        <v>31</v>
+      </c>
+      <c r="B71" s="1">
+        <v>50716</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>181</v>
       </c>
       <c r="D71">
         <v>0</v>
       </c>
-      <c r="E71">
-        <v>1</v>
+      <c r="E71" s="1">
+        <v>2866</v>
       </c>
       <c r="F71">
-        <v>7.0000000000000001E-3</v>
+        <v>0.96799999999999997</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B72">
         <v>2</v>
@@ -2911,10 +2983,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B73">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -2923,18 +2995,18 @@
         <v>0</v>
       </c>
       <c r="E73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73">
-        <v>1.7999999999999999E-2</v>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B74">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -2943,49 +3015,69 @@
         <v>0</v>
       </c>
       <c r="E74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F74">
-        <v>4.0000000000000001E-3</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B75">
-        <v>577</v>
+        <v>1</v>
       </c>
       <c r="C75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D75">
         <v>0</v>
       </c>
       <c r="E75">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="F75">
-        <v>0.36099999999999999</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
+        <v>36</v>
+      </c>
+      <c r="B76">
+        <v>577</v>
+      </c>
+      <c r="C76">
+        <v>2</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>48</v>
+      </c>
+      <c r="F76">
+        <v>0.36099999999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>37</v>
       </c>
-      <c r="B76">
+      <c r="B77">
         <v>2</v>
       </c>
-      <c r="C76">
-        <v>0</v>
-      </c>
-      <c r="D76">
-        <v>0</v>
-      </c>
-      <c r="E76">
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
         <v>2</v>
       </c>
-      <c r="F76">
+      <c r="F77">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
@@ -2996,648 +3088,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D9E34E6-D0FD-41D4-8E60-9276E15A3FED}">
-  <dimension ref="A1:G32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2">
-        <v>595271</v>
-      </c>
-      <c r="D2">
-        <f t="shared" ref="D2:D32" si="0">C2/$G$2</f>
-        <v>0.33356120975482928</v>
-      </c>
-      <c r="E2">
-        <f>D2</f>
-        <v>0.33356120975482928</v>
-      </c>
-      <c r="G2">
-        <f>SUM(C2:C32)</f>
-        <v>1784593</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3">
-        <v>251131</v>
-      </c>
-      <c r="D3">
-        <f t="shared" si="0"/>
-        <v>0.14072172198366797</v>
-      </c>
-      <c r="E3">
-        <f>E2+D3</f>
-        <v>0.47428293173849723</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4">
-        <v>231000</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>0.12944127876776385</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E32" si="1">E3+D4</f>
-        <v>0.60372421050626102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5">
-        <v>182323</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>0.10216503146655848</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="1"/>
-        <v>0.70588924197281955</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6">
-        <v>172310</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>9.6554228331053635E-2</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="1"/>
-        <v>0.8024434703038732</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7">
-        <v>139952</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>7.8422362970156215E-2</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="1"/>
-        <v>0.88086583327402945</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8">
-        <v>77433</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>4.338972527629549E-2</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="1"/>
-        <v>0.92425555855032493</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9">
-        <v>50716</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>2.8418804735869746E-2</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="1"/>
-        <v>0.9526743632861947</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10">
-        <v>32575</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>1.8253461713679253E-2</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="1"/>
-        <v>0.97092782499987396</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11">
-        <v>32055</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>1.796207874848775E-2</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="1"/>
-        <v>0.98888990374836172</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12">
-        <v>8983</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>5.0336407236832147E-3</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="1"/>
-        <v>0.9939235444720449</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13">
-        <v>7318</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>4.1006548832142678E-3</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="1"/>
-        <v>0.99802419935525921</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14">
-        <v>950</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>5.3233426333063061E-4</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>0.99855653361858987</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15">
-        <v>845</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>4.7349731843619248E-4</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
-        <v>0.99903003093702603</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16">
-        <v>577</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>3.2332302099134086E-4</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="1"/>
-        <v>0.99935335395801739</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17">
-        <v>530</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>2.9698648375287809E-4</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="1"/>
-        <v>0.99965034044177026</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18">
-        <v>487</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>2.7289135393896536E-4</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="1"/>
-        <v>0.99992323179570919</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19">
-        <v>53</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>2.9698648375287812E-5</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="1"/>
-        <v>0.99995293044408451</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20">
-        <v>32</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>1.7931259396400188E-5</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="1"/>
-        <v>0.99997086170348093</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>81</v>
-      </c>
-      <c r="B21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21">
-        <v>19</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>1.0646685266612612E-5</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="1"/>
-        <v>0.99998150838874755</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>86</v>
-      </c>
-      <c r="B22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22">
-        <v>9</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>5.043166705237553E-6</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="1"/>
-        <v>0.9999865515554528</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>89</v>
-      </c>
-      <c r="B23" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23">
-        <v>6</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="0"/>
-        <v>3.3621111368250352E-6</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="1"/>
-        <v>0.99998991366658962</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>84</v>
-      </c>
-      <c r="B24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24">
-        <v>4</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="0"/>
-        <v>2.2414074245500235E-6</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="1"/>
-        <v>0.99999215507401418</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="0"/>
-        <v>1.6810555684125176E-6</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="1"/>
-        <v>0.99999383612958259</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>91</v>
-      </c>
-      <c r="B26" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
-        <v>1.1207037122750117E-6</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="1"/>
-        <v>0.99999495683329487</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>88</v>
-      </c>
-      <c r="B27" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="0"/>
-        <v>1.1207037122750117E-6</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="1"/>
-        <v>0.99999607753700714</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>87</v>
-      </c>
-      <c r="B28" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="0"/>
-        <v>1.1207037122750117E-6</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="1"/>
-        <v>0.99999719824071942</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>83</v>
-      </c>
-      <c r="B29" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="0"/>
-        <v>1.1207037122750117E-6</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="1"/>
-        <v>0.9999983189444317</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>90</v>
-      </c>
-      <c r="B30" t="s">
-        <v>67</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30">
-        <f t="shared" si="0"/>
-        <v>5.6035185613750587E-7</v>
-      </c>
-      <c r="E30">
-        <f t="shared" si="1"/>
-        <v>0.99999887929628783</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>85</v>
-      </c>
-      <c r="B31" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31">
-        <f t="shared" si="0"/>
-        <v>5.6035185613750587E-7</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="1"/>
-        <v>0.99999943964814397</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>78</v>
-      </c>
-      <c r="B32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32">
-        <f t="shared" si="0"/>
-        <v>5.6035185613750587E-7</v>
-      </c>
-      <c r="E32">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C32">
-    <sortCondition descending="1" ref="C2:C32"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{087AE925-B5C9-4354-81CB-BC835F925237}">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3671,25 +3125,25 @@
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="28"/>
+      <c r="D2" s="29"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="G2" s="28"/>
+      <c r="G2" s="29"/>
       <c r="H2" s="11"/>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="J2" s="28"/>
+      <c r="J2" s="29"/>
       <c r="K2" s="11"/>
-      <c r="L2" s="28" t="s">
+      <c r="L2" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="M2" s="28"/>
+      <c r="M2" s="29"/>
       <c r="N2" s="11"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -4207,102 +3661,102 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="30">
         <v>0.6</v>
       </c>
-      <c r="D18" s="20">
+      <c r="D18" s="31">
         <v>0.496</v>
       </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="14">
+      <c r="E18" s="22"/>
+      <c r="F18" s="30">
         <v>0.5</v>
       </c>
-      <c r="G18" s="20">
+      <c r="G18" s="31">
         <v>0.85499999999999998</v>
       </c>
-      <c r="H18" s="15"/>
-      <c r="I18" s="14">
+      <c r="H18" s="22"/>
+      <c r="I18" s="30">
         <v>-1.6</v>
       </c>
-      <c r="J18" s="20">
+      <c r="J18" s="31">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="K18" s="11"/>
-      <c r="L18" s="24">
+      <c r="K18" s="21"/>
+      <c r="L18" s="32">
         <v>-0.04</v>
       </c>
-      <c r="M18" s="15">
+      <c r="M18" s="22">
         <v>0.155</v>
       </c>
       <c r="N18" s="11"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="33">
         <v>13.6</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19" s="34">
         <v>1.4E-2</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="19">
+      <c r="E19" s="22"/>
+      <c r="F19" s="33">
         <v>50.4</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19" s="34">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="H19" s="15"/>
-      <c r="I19" s="19">
+      <c r="H19" s="22"/>
+      <c r="I19" s="33">
         <v>17.600000000000001</v>
       </c>
-      <c r="J19" s="25">
+      <c r="J19" s="34">
         <v>2E-3</v>
       </c>
-      <c r="K19" s="11"/>
-      <c r="L19" s="26">
+      <c r="K19" s="21"/>
+      <c r="L19" s="35">
         <v>-0.04</v>
       </c>
-      <c r="M19" s="27">
+      <c r="M19" s="36">
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="N19" s="11"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="37">
         <v>0.2</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="38">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="14">
+      <c r="E20" s="28"/>
+      <c r="F20" s="37">
         <v>-0.1</v>
       </c>
-      <c r="G20" s="20">
+      <c r="G20" s="38">
         <v>0.82099999999999995</v>
       </c>
-      <c r="H20" s="15"/>
-      <c r="I20" s="14">
+      <c r="H20" s="28"/>
+      <c r="I20" s="37">
         <v>0.1</v>
       </c>
-      <c r="J20" s="20">
+      <c r="J20" s="38">
         <v>0.20699999999999999</v>
       </c>
-      <c r="K20" s="11"/>
-      <c r="L20" s="24">
+      <c r="K20" s="8"/>
+      <c r="L20" s="39">
         <v>-0.06</v>
       </c>
-      <c r="M20" s="15">
+      <c r="M20" s="28">
         <v>0.159</v>
       </c>
       <c r="N20" s="11"/>
@@ -4348,6 +3802,642 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D9E34E6-D0FD-41D4-8E60-9276E15A3FED}">
+  <dimension ref="A1:G32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>595271</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D32" si="0">C2/$G$2</f>
+        <v>0.33356120975482928</v>
+      </c>
+      <c r="E2">
+        <f>D2</f>
+        <v>0.33356120975482928</v>
+      </c>
+      <c r="G2">
+        <f>SUM(C2:C32)</f>
+        <v>1784593</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3">
+        <v>251131</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>0.14072172198366797</v>
+      </c>
+      <c r="E3">
+        <f>E2+D3</f>
+        <v>0.47428293173849723</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4">
+        <v>231000</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.12944127876776385</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E32" si="1">E3+D4</f>
+        <v>0.60372421050626102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5">
+        <v>182323</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.10216503146655848</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>0.70588924197281955</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <v>172310</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>9.6554228331053635E-2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>0.8024434703038732</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7">
+        <v>139952</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>7.8422362970156215E-2</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>0.88086583327402945</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8">
+        <v>77433</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>4.338972527629549E-2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>0.92425555855032493</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9">
+        <v>50716</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>2.8418804735869746E-2</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>0.9526743632861947</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10">
+        <v>32575</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1.8253461713679253E-2</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>0.97092782499987396</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11">
+        <v>32055</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>1.796207874848775E-2</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>0.98888990374836172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12">
+        <v>8983</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>5.0336407236832147E-3</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>0.9939235444720449</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13">
+        <v>7318</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>4.1006548832142678E-3</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>0.99802419935525921</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14">
+        <v>950</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>5.3233426333063061E-4</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>0.99855653361858987</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15">
+        <v>845</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>4.7349731843619248E-4</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>0.99903003093702603</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16">
+        <v>577</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>3.2332302099134086E-4</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>0.99935335395801739</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17">
+        <v>530</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>2.9698648375287809E-4</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>0.99965034044177026</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18">
+        <v>487</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>2.7289135393896536E-4</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>0.99992323179570919</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19">
+        <v>53</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>2.9698648375287812E-5</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>0.99995293044408451</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20">
+        <v>32</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>1.7931259396400188E-5</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>0.99997086170348093</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21">
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>1.0646685266612612E-5</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>0.99998150838874755</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22">
+        <v>9</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>5.043166705237553E-6</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>0.9999865515554528</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>3.3621111368250352E-6</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>0.99998991366658962</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>2.2414074245500235E-6</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>0.99999215507401418</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>1.6810555684125176E-6</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>0.99999383612958259</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>1.1207037122750117E-6</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>0.99999495683329487</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>1.1207037122750117E-6</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>0.99999607753700714</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>1.1207037122750117E-6</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>0.99999719824071942</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>1.1207037122750117E-6</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>0.9999983189444317</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>5.6035185613750587E-7</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>0.99999887929628783</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>5.6035185613750587E-7</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>0.99999943964814397</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>5.6035185613750587E-7</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C32">
+    <sortCondition descending="1" ref="C2:C32"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -4642,8 +4732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB20FAA-A8B7-4843-8873-9609280C8D71}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D38" sqref="B36:D38"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4665,10 +4755,10 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="28"/>
+      <c r="D2" s="29"/>
       <c r="E2" s="21"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -4801,10 +4891,10 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="D13" s="28"/>
+      <c r="D13" s="29"/>
       <c r="E13" s="21"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -4895,10 +4985,10 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="D21" s="28"/>
+      <c r="D21" s="29"/>
       <c r="E21" s="21"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -5041,10 +5131,10 @@
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="D33" s="28"/>
+      <c r="D33" s="29"/>
       <c r="E33" s="22"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>